<commit_message>
cap nhat du lieu hang ngay
</commit_message>
<xml_diff>
--- a/2023/PhaiSinh.xlsx
+++ b/2023/PhaiSinh.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/Desktop/stocks/App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/Documents/github/ssh/stocks/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A129FE52-7743-8D41-BB1B-E4D17B16D3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3694DA6-A73D-B945-9D31-8566E453CB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16860" xr2:uid="{C3A8CAD2-D0D3-0E42-AE62-C721C0509473}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16860" activeTab="2" xr2:uid="{C3A8CAD2-D0D3-0E42-AE62-C721C0509473}"/>
   </bookViews>
   <sheets>
     <sheet name="MoneyFlow" sheetId="3" r:id="rId1"/>
@@ -7060,9 +7060,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7100,7 +7100,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7206,7 +7206,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7348,7 +7348,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7359,7 +7359,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A88:AD152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="69" workbookViewId="0">
+    <sheetView zoomScale="69" workbookViewId="0">
       <selection activeCell="W30" sqref="W30"/>
     </sheetView>
   </sheetViews>
@@ -17506,7 +17506,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>

</xml_diff>